<commit_message>
Doctor menu design has changed
</commit_message>
<xml_diff>
--- a/doc/Doctors_Permissions.xlsx
+++ b/doc/Doctors_Permissions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>#</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>doctor_12.php</t>
+  </si>
+  <si>
+    <t>Lusines</t>
+  </si>
+  <si>
+    <t>Armines</t>
+  </si>
+  <si>
+    <t>Anahits</t>
+  </si>
+  <si>
+    <t>Melina</t>
   </si>
 </sst>
 </file>
@@ -138,7 +150,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +160,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -249,6 +279,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -267,6 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,34 +594,34 @@
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
@@ -604,14 +637,14 @@
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -622,18 +655,19 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="11" t="s">
         <v>22</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="14">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -644,16 +678,17 @@
       <c r="F4" s="4"/>
       <c r="G4" s="3"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="11"/>
+      <c r="I4" s="13"/>
       <c r="J4" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="14">
         <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -664,16 +699,17 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="11"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="14">
         <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -684,16 +720,17 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="11"/>
+      <c r="I6" s="13"/>
       <c r="J6" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="14">
         <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -704,16 +741,17 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="11"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="14">
         <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -724,16 +762,17 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="14">
         <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -744,16 +783,17 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="11"/>
+      <c r="I9" s="13"/>
       <c r="J9" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="14">
         <v>65</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -764,16 +804,17 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="13"/>
       <c r="J10" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="14">
         <v>162</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -784,16 +825,17 @@
       <c r="F11" s="4"/>
       <c r="G11" s="3"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="11"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="14">
         <v>270</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -804,16 +846,17 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="11"/>
+      <c r="I12" s="13"/>
       <c r="J12" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="14">
         <v>390</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -824,12 +867,13 @@
       <c r="F13" s="4"/>
       <c r="G13" s="3"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="11"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -844,96 +888,185 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="10"/>
+      <c r="I14" s="13"/>
       <c r="J14" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="4">
-        <v>14</v>
+        <v>484</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="I15" s="13"/>
       <c r="J15" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="4">
-        <v>15</v>
+        <v>486</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="11"/>
+      <c r="I16" s="13"/>
       <c r="J16" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>29</v>
+        <v>488</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="11"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="4">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="10"/>
+      <c r="I18" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="J18" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5" t="s">
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>16</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <v>38</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -948,8 +1081,8 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="I3:I14"/>
-    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="I3:I17"/>
+    <mergeCell ref="I18:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>